<commit_message>
update research and planning on data/ETL pipeline architecture
</commit_message>
<xml_diff>
--- a/column_mapping_btw_analytics_and_oracle_tables.xlsx
+++ b/column_mapping_btw_analytics_and_oracle_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abgov-my.sharepoint.com/personal/kai_wong_gov_ab_ca/Documents/_work/project/etl_for_ecollision_fusion_database/etl-for-ecol-fusion-database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="393" documentId="8_{23D0BAB7-18E8-4959-9F4E-FFA96A3ED94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB0E09E9-7ECB-416C-A8F2-F0BAF05778A9}"/>
+  <xr:revisionPtr revIDLastSave="396" documentId="8_{23D0BAB7-18E8-4959-9F4E-FFA96A3ED94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DB61988-D662-4DED-A8DF-8BA59128FA72}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{FB73D8E5-4A8D-4C49-9DB8-09C218E8D022}"/>
+    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{FB73D8E5-4A8D-4C49-9DB8-09C218E8D022}"/>
   </bookViews>
   <sheets>
     <sheet name="table - collisions" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2244" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2244" uniqueCount="365">
   <si>
     <t>original database:</t>
   </si>
@@ -1137,6 +1137,9 @@
   </si>
   <si>
     <t>perfect match</t>
+  </si>
+  <si>
+    <t>Yes (a duplicate column named LOC_HWY_NBR on collisions table)</t>
   </si>
 </sst>
 </file>
@@ -7958,9 +7961,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5F9DAB-6992-41EF-B70B-DC9000CCE65E}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8164,7 +8167,7 @@
       <c r="E9" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="4" t="s">
         <v>334</v>
       </c>
       <c r="H9" t="s">
@@ -8174,7 +8177,7 @@
         <v>150</v>
       </c>
       <c r="J9" t="s">
-        <v>150</v>
+        <v>364</v>
       </c>
       <c r="K9" t="s">
         <v>347</v>
@@ -8747,7 +8750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B4E32B-3AEC-4A84-B2D5-13C754A4FDE8}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
     </sheetView>

</xml_diff>

<commit_message>
finalize setting for "official" ingestion
</commit_message>
<xml_diff>
--- a/column_mapping_btw_analytics_and_oracle_tables.xlsx
+++ b/column_mapping_btw_analytics_and_oracle_tables.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="396" documentId="8_{23D0BAB7-18E8-4959-9F4E-FFA96A3ED94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DB61988-D662-4DED-A8DF-8BA59128FA72}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{FB73D8E5-4A8D-4C49-9DB8-09C218E8D022}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FB73D8E5-4A8D-4C49-9DB8-09C218E8D022}"/>
   </bookViews>
   <sheets>
     <sheet name="table - collisions" sheetId="1" r:id="rId1"/>
@@ -1513,23 +1513,23 @@
   <dimension ref="A1:N129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I106" sqref="I106"/>
+      <pane ySplit="5" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" customWidth="1"/>
+    <col min="9" max="9" width="23.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>131</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>109</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>126</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>94</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>118</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>119</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>121</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>110</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>112</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>106</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>132</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>41</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>45</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>81</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>24</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>87</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>116</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>89</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>91</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>90</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>44</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>115</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>82</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>84</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>122</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>47</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>103</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>98</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>69</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>68</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>130</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>53</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>73</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>99</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>61</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>123</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>101</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>20</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>102</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>16</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>64</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>9</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>77</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>78</v>
       </c>
@@ -3826,7 +3826,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>19</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>38</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>40</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>111</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>92</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>32</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>128</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>97</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>127</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>114</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>62</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>27</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>28</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>117</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>29</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>22</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>25</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>13</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>14</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>26</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>57</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>120</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>129</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>34</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>93</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>79</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>59</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>15</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>70</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>107</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>108</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>37</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>52</v>
       </c>
@@ -4579,22 +4579,22 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>178</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>179</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>180</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>181</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>182</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>183</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>184</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>185</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>196</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>197</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>198</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>186</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>187</v>
       </c>
@@ -5227,7 +5227,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>188</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>189</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>199</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>190</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>201</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>191</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>192</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>193</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>194</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>195</v>
       </c>
@@ -5495,23 +5495,23 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5559,7 +5559,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>210</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>211</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>212</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>214</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>215</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>216</v>
       </c>
@@ -5773,7 +5773,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>218</v>
       </c>
@@ -5819,7 +5819,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -5842,7 +5842,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>219</v>
       </c>
@@ -5888,7 +5888,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>220</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>221</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>222</v>
       </c>
@@ -5963,7 +5963,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>223</v>
       </c>
@@ -5986,7 +5986,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>224</v>
       </c>
@@ -6009,7 +6009,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>225</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>226</v>
       </c>
@@ -6055,7 +6055,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>227</v>
       </c>
@@ -6078,7 +6078,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>228</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>229</v>
       </c>
@@ -6124,7 +6124,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>230</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -6170,7 +6170,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>231</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>232</v>
       </c>
@@ -6216,7 +6216,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>233</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>234</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>235</v>
       </c>
@@ -6285,7 +6285,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>236</v>
       </c>
@@ -6308,7 +6308,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>98</v>
       </c>
@@ -6331,7 +6331,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>130</v>
       </c>
@@ -6406,7 +6406,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>237</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -6452,7 +6452,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>238</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>239</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>240</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>241</v>
       </c>
@@ -6544,7 +6544,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>242</v>
       </c>
@@ -6567,7 +6567,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>243</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>244</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>245</v>
       </c>
@@ -6636,7 +6636,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>246</v>
       </c>
@@ -6659,7 +6659,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>248</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>199</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>249</v>
       </c>
@@ -6757,7 +6757,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>250</v>
       </c>
@@ -6780,7 +6780,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>251</v>
       </c>
@@ -6803,7 +6803,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>252</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>253</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>254</v>
       </c>
@@ -6882,23 +6882,23 @@
   <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>268</v>
       </c>
@@ -7007,7 +7007,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>269</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>270</v>
       </c>
@@ -7053,7 +7053,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -7099,7 +7099,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>272</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>273</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>274</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>275</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>276</v>
       </c>
@@ -7243,7 +7243,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -7266,7 +7266,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>277</v>
       </c>
@@ -7295,7 +7295,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>278</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>279</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>280</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>281</v>
       </c>
@@ -7393,7 +7393,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>282</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>283</v>
       </c>
@@ -7439,7 +7439,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>284</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>285</v>
       </c>
@@ -7485,7 +7485,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>286</v>
       </c>
@@ -7508,7 +7508,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>98</v>
       </c>
@@ -7531,7 +7531,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -7577,7 +7577,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>130</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -7629,7 +7629,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>287</v>
       </c>
@@ -7652,7 +7652,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>288</v>
       </c>
@@ -7675,7 +7675,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>289</v>
       </c>
@@ -7698,7 +7698,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>290</v>
       </c>
@@ -7721,7 +7721,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>199</v>
       </c>
@@ -7750,7 +7750,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -7779,7 +7779,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>291</v>
       </c>
@@ -7802,7 +7802,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>292</v>
       </c>
@@ -7825,7 +7825,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>293</v>
       </c>
@@ -7842,7 +7842,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>294</v>
       </c>
@@ -7859,7 +7859,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>295</v>
       </c>
@@ -7876,7 +7876,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>296</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>297</v>
       </c>
@@ -7916,7 +7916,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>298</v>
       </c>
@@ -7933,7 +7933,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>299</v>
       </c>
@@ -7963,22 +7963,22 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -8026,7 +8026,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -8061,7 +8061,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>331</v>
       </c>
@@ -8096,7 +8096,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>332</v>
       </c>
@@ -8125,7 +8125,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>179</v>
       </c>
@@ -8154,7 +8154,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>314</v>
       </c>
@@ -8183,7 +8183,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>315</v>
       </c>
@@ -8212,7 +8212,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>316</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -8270,7 +8270,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -8299,7 +8299,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>318</v>
       </c>
@@ -8328,7 +8328,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>319</v>
       </c>
@@ -8357,7 +8357,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>333</v>
       </c>
@@ -8386,7 +8386,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>334</v>
       </c>
@@ -8415,7 +8415,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>335</v>
       </c>
@@ -8444,7 +8444,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>336</v>
       </c>
@@ -8473,7 +8473,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>320</v>
       </c>
@@ -8502,7 +8502,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>321</v>
       </c>
@@ -8516,7 +8516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>337</v>
       </c>
@@ -8530,7 +8530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -8544,7 +8544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -8572,7 +8572,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -8586,7 +8586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>338</v>
       </c>
@@ -8600,7 +8600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -8614,7 +8614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>322</v>
       </c>
@@ -8628,7 +8628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>323</v>
       </c>
@@ -8636,7 +8636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>339</v>
       </c>
@@ -8644,7 +8644,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>324</v>
       </c>
@@ -8652,7 +8652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>340</v>
       </c>
@@ -8660,7 +8660,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>341</v>
       </c>
@@ -8668,7 +8668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>342</v>
       </c>
@@ -8676,7 +8676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>325</v>
       </c>
@@ -8684,7 +8684,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>343</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>344</v>
       </c>
@@ -8700,7 +8700,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>345</v>
       </c>
@@ -8708,7 +8708,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>327</v>
       </c>
@@ -8716,7 +8716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>328</v>
       </c>
@@ -8724,7 +8724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>329</v>
       </c>
@@ -8732,7 +8732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>330</v>
       </c>
@@ -8752,22 +8752,22 @@
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
+      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8781,7 +8781,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8795,7 +8795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -8815,7 +8815,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -8852,7 +8852,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>355</v>
       </c>
@@ -8879,7 +8879,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>356</v>
       </c>
@@ -8901,7 +8901,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>357</v>
       </c>
@@ -8923,7 +8923,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -8945,7 +8945,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -8967,7 +8967,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -8989,7 +8989,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>358</v>
       </c>
@@ -9011,7 +9011,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>359</v>
       </c>
@@ -9033,7 +9033,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -9055,7 +9055,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -9077,7 +9077,7 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -9099,7 +9099,7 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -9121,7 +9121,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>360</v>
       </c>
@@ -9143,7 +9143,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>361</v>
       </c>
@@ -9165,7 +9165,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>362</v>
       </c>

</xml_diff>